<commit_message>
NSE Options v2 after correction of lower and upper band
</commit_message>
<xml_diff>
--- a/outputs/Masters.xlsx
+++ b/outputs/Masters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NSE\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FE893D-005C-47F0-90C6-6B228F5108BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0711FA2-0164-4058-85FD-9018798A6BAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4116" yWindow="2280" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>date</t>
   </si>
@@ -28,16 +28,28 @@
     <t>time</t>
   </si>
   <si>
+    <t>script</t>
+  </si>
+  <si>
     <t>base_strike</t>
   </si>
   <si>
-    <t>current_nifty</t>
-  </si>
-  <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>order_strike</t>
+    <t>ltp</t>
+  </si>
+  <si>
+    <t>base_change</t>
+  </si>
+  <si>
+    <t>current_change</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>call_put</t>
+  </si>
+  <si>
+    <t>buy_sell</t>
   </si>
   <si>
     <t>call_price</t>
@@ -46,10 +58,13 @@
     <t>put_price</t>
   </si>
   <si>
-    <t>call_put</t>
-  </si>
-  <si>
-    <t>buy_sell</t>
+    <t>total_premium</t>
+  </si>
+  <si>
+    <t>cumm_premium</t>
+  </si>
+  <si>
+    <t>amt</t>
   </si>
   <si>
     <t>executed</t>
@@ -58,25 +73,43 @@
     <t>remarks</t>
   </si>
   <si>
+    <t>kount</t>
+  </si>
+  <si>
+    <t>sum_amt</t>
+  </si>
+  <si>
+    <t>sum_qty</t>
+  </si>
+  <si>
+    <t>qty_strike</t>
+  </si>
+  <si>
+    <t>cum_qty_strike</t>
+  </si>
+  <si>
+    <t>arrived_strike</t>
+  </si>
+  <si>
     <t>lower_band</t>
   </si>
   <si>
     <t>upper_band</t>
   </si>
   <si>
-    <t>23-Aug-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>08:54:47</t>
-  </si>
-  <si>
-    <t>08:56:30</t>
-  </si>
-  <si>
-    <t>09:09:45</t>
+    <t>03-Sep-2019</t>
+  </si>
+  <si>
+    <t>11:19:43</t>
+  </si>
+  <si>
+    <t>11:20:03</t>
+  </si>
+  <si>
+    <t>11:21:10</t>
+  </si>
+  <si>
+    <t>SBIN</t>
   </si>
   <si>
     <t>CALL</t>
@@ -85,7 +118,7 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>S</t>
+    <t>SELL</t>
   </si>
   <si>
     <t>Y</t>
@@ -97,10 +130,10 @@
     <t>First PUT Order</t>
   </si>
   <si>
-    <t>NIFTY is DOWN</t>
-  </si>
-  <si>
-    <t>Average</t>
+    <t>CALL Order</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -512,30 +545,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -578,225 +622,346 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>10750</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="1">
-        <v>10741.35</v>
+        <v>320</v>
       </c>
       <c r="E2" s="1">
-        <v>8.65</v>
+        <v>269.35000000000002</v>
       </c>
       <c r="F2" s="1">
-        <v>10750</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
-        <v>90</v>
+        <v>-50.65</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>10660</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>10840</v>
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="U2" s="1">
+        <v>960000</v>
+      </c>
+      <c r="V2" s="1">
+        <v>960000</v>
+      </c>
+      <c r="W2" s="1">
+        <v>320</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10750</v>
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D3" s="1">
-        <v>10741.35</v>
+        <v>320</v>
       </c>
       <c r="E3" s="1">
-        <v>8.65</v>
+        <v>269.35000000000002</v>
       </c>
       <c r="F3" s="1">
-        <v>10750</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>-50.65</v>
       </c>
       <c r="H3" s="1">
-        <v>105.55</v>
+        <v>3000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>10554.45</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>10945.55</v>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="U3" s="1">
+        <v>960000</v>
+      </c>
+      <c r="V3" s="1">
+        <v>960000</v>
+      </c>
+      <c r="W3" s="1">
+        <v>320</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10750</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="1">
-        <v>10741.35</v>
+        <v>320</v>
       </c>
       <c r="E4" s="1">
-        <v>8.65</v>
+        <v>269.35000000000002</v>
       </c>
       <c r="F4" s="1">
-        <v>10750</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
-        <v>85</v>
+        <v>-50.65</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>6000</v>
+      </c>
+      <c r="U4" s="1">
+        <v>960000</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1920000</v>
+      </c>
+      <c r="W4" s="1">
+        <v>320</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="1">
-        <v>10469.450000000001</v>
-      </c>
-      <c r="N4" s="1">
-        <v>11030.55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10750</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="1">
-        <v>10741.35</v>
+        <v>320</v>
       </c>
       <c r="E5" s="1">
-        <v>8.65</v>
+        <v>269.3</v>
       </c>
       <c r="F5" s="1">
-        <v>10750</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1">
-        <v>90</v>
+        <v>-50.7</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>10379.450000000001</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>11120.55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="1">
-        <v>10515.84</v>
-      </c>
-      <c r="N6" s="1">
-        <v>10984.16</v>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>9000</v>
+      </c>
+      <c r="U5" s="1">
+        <v>960000</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2880000</v>
+      </c>
+      <c r="W5" s="1">
+        <v>320</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>